<commit_message>
Metadata change + fresh Omeka import spreadsheet
</commit_message>
<xml_diff>
--- a/XQuery/OmekaData_2015Exhibits.xlsx
+++ b/XQuery/OmekaData_2015Exhibits.xlsx
@@ -10,7 +10,7 @@
     <sheet name="OmekaData_2015Exhibits" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OmekaData_2015Exhibits!$A$1:$L$343</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OmekaData_2015Exhibits!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1060,7 +1060,7 @@
     <t>Shadow (Fictitious character)</t>
   </si>
   <si>
-    <t>"Who knows what evil lurks in the hearts of men? The Shadow knows!" These words, spoken by Walter B. Gibson's fictional crime-fighting vigilante The Shadow are part of radio history. The Shadow debuted on the 1930 CBS radio show, Detective Story Hour, and quickly built a fan base, as The Shadow, alias Lamont Cranston, helped police fight crime with his psychic powers of invisibility. The show ran for 20 years and continues to be popular in re-broadcasts such as this, featuring Orson Wells.</t>
+    <t>"Who knows what evil lurks in the hearts of men? The Shadow knows!” These words, spoken by Walter B. Gibson's fictional crime-fighting vigilante The Shadow are part of radio history. The Shadow debuted on the 1930 CBS radio show, Detective Story Hour, and quickly built a fan base, as The Shadow, alias Lamont Cranston, helped police fight crime with his psychic powers of invisibility. The show ran for 20 years and continues to be popular in re-broadcasts such as this, featuring Orson Wells.</t>
   </si>
   <si>
     <t>Work: Company is defunct with no forwarding information. Using small amount of material for transformative use; no negative effect on market.|Image: Copyright maintained by Vanderbilt University Special Collections</t>
@@ -1519,7 +1519,7 @@
     <t>First introduced in 1900, the Kodak Brownie camera sold for only $1.00, and allowed users to make photos easily and cheaply.  Brownies were portable and recorded people as they were and as they wanted to be seen at the beach, at Coney Island, on a downtown streetcar or automobile.  Kodak’s slogan was “You press the button, we do the rest”.</t>
   </si>
   <si>
-    <t>Loan from private collection</t>
+    <t>On Loan from the Collection of Pamela J. Morgan</t>
   </si>
   <si>
     <t>Work: Lender granted copyright.|Image: Copyright maintained by Vanderbilt University Special Collections</t>
@@ -8946,9 +8946,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9295,50 +9296,60 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" customWidth="1"/>
+    <col min="6" max="6" width="64.28515625" customWidth="1"/>
+    <col min="7" max="7" width="72" customWidth="1"/>
+    <col min="8" max="8" width="74.5703125" customWidth="1"/>
+    <col min="9" max="9" width="104.28515625" customWidth="1"/>
+    <col min="10" max="10" width="34.85546875" customWidth="1"/>
+    <col min="11" max="11" width="57.28515625" customWidth="1"/>
+    <col min="12" max="12" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -21781,7 +21792,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L343"/>
+  <autoFilter ref="A1:L1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
XQuery: Creation vs publication date labeling, removed Filename field from csv. Minor VRA/Omeka documentation changes.
</commit_message>
<xml_diff>
--- a/XQuery/OmekaData_2015Exhibits.xlsx
+++ b/XQuery/OmekaData_2015Exhibits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="11565"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="OmekaData_2015Exhibits" sheetId="1" r:id="rId1"/>
@@ -22,28 +22,28 @@
     <t>BASE_URI</t>
   </si>
   <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>FORMAT</t>
-  </si>
-  <si>
-    <t>CONTRIBUTOR</t>
-  </si>
-  <si>
-    <t>SUBJECT</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>RIGHTS</t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Rights</t>
   </si>
   <si>
     <t>FILE_PATH</t>
@@ -2935,7 +2935,7 @@
     <t>Nahum N. Glatzer, a disciple of Franz Rosenzweig, succeeded Martin Buber in his chair at the University of Frankfurt in 1932. Glazter moved to the United States in 1938 and, after a series of academic posts, began teaching at Brandeis University in 1950. He wrote on the history of rabbinic Judaism as well as contemporary Jewry.</t>
   </si>
   <si>
-    <t>http://www.jewishfilm.org/Catalogue/films/nahumglatzer.htm</t>
+    <t>Online resource, available via: http://www.jewishfilm.org/Catalogue/films/nahumglatzer.htm</t>
   </si>
   <si>
     <t>http://libexh.library.vanderbilt.edu/impomeka/2015-exhibit/Glatzer1.jpg</t>
@@ -8432,16 +8432,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" customWidth="1"/>
-    <col min="9" max="9" width="70.42578125" customWidth="1"/>
-    <col min="12" max="12" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>